<commit_message>
table and solution update
</commit_message>
<xml_diff>
--- a/Grid_5x5/Solutions/Solution_NDP_S005/Spreadsheet/VIS17_PuTAss_CapaRestNo_InterlYes_v04.xlsx
+++ b/Grid_5x5/Solutions/Solution_NDP_S005/Spreadsheet/VIS17_PuTAss_CapaRestNo_InterlYes_v04.xlsx
@@ -2590,7 +2590,7 @@
         <v>166</v>
       </c>
       <c r="C39" s="38">
-        <v>20.695569351993193</v>
+        <v>20.695569351993196</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>129</v>
@@ -2610,7 +2610,7 @@
         <v>200</v>
       </c>
       <c r="C40" s="39">
-        <v>21.262706707235676</v>
+        <v>21.262706707235679</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>129</v>
@@ -2630,7 +2630,7 @@
         <v>201</v>
       </c>
       <c r="C41" s="39">
-        <v>0.28758683353967979</v>
+        <v>0.28758683353967984</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>42</v>
@@ -2651,7 +2651,7 @@
         <v>202</v>
       </c>
       <c r="C42" s="39">
-        <v>0.91484404761904781</v>
+        <v>0.91484404761904736</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>42</v>
@@ -2671,7 +2671,7 @@
         <v>204</v>
       </c>
       <c r="C43" s="40">
-        <v>1.1153857142857142</v>
+        <v>1.1153857142857144</v>
       </c>
       <c r="D43" s="67" t="s">
         <v>42</v>
@@ -8858,7 +8858,7 @@
         <v>68.527000000000001</v>
       </c>
       <c r="M28" s="72">
-        <v>77.42</v>
+        <v>77.419999999999987</v>
       </c>
       <c r="N28" s="72">
         <v>109.315</v>
@@ -8896,13 +8896,13 @@
         <v>70</v>
       </c>
       <c r="K29" s="72">
-        <v>42.225000000000001</v>
+        <v>42.225000000000009</v>
       </c>
       <c r="L29" s="72">
-        <v>88.448000000000008</v>
+        <v>88.447999999999993</v>
       </c>
       <c r="M29" s="72">
-        <v>20.866999999999997</v>
+        <v>20.867000000000001</v>
       </c>
       <c r="N29" s="72">
         <v>130.673</v>
@@ -9060,7 +9060,7 @@
         <v>70</v>
       </c>
       <c r="K33" s="72">
-        <v>134.74099999999999</v>
+        <v>134.74100000000001</v>
       </c>
       <c r="L33" s="72">
         <v>0</v>
@@ -9069,7 +9069,7 @@
         <v>0</v>
       </c>
       <c r="N33" s="72">
-        <v>134.74099999999999</v>
+        <v>134.74100000000001</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -9104,7 +9104,7 @@
         <v>70</v>
       </c>
       <c r="K34" s="72">
-        <v>31.315000000000005</v>
+        <v>31.315000000000001</v>
       </c>
       <c r="L34" s="72">
         <v>125.38800000000001</v>
@@ -9151,13 +9151,13 @@
         <v>32.918000000000006</v>
       </c>
       <c r="L35" s="72">
-        <v>116.99900000000002</v>
+        <v>116.999</v>
       </c>
       <c r="M35" s="72">
-        <v>39.704000000000008</v>
+        <v>39.704000000000001</v>
       </c>
       <c r="N35" s="72">
-        <v>149.91700000000003</v>
+        <v>149.917</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -9192,16 +9192,16 @@
         <v>70</v>
       </c>
       <c r="K36" s="72">
-        <v>33.498000000000005</v>
+        <v>33.497999999999998</v>
       </c>
       <c r="L36" s="72">
-        <v>107.354</v>
+        <v>107.35399999999998</v>
       </c>
       <c r="M36" s="72">
         <v>42.563000000000002</v>
       </c>
       <c r="N36" s="72">
-        <v>140.852</v>
+        <v>140.85199999999998</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -9242,7 +9242,7 @@
         <v>64.491</v>
       </c>
       <c r="M37" s="72">
-        <v>76.361000000000004</v>
+        <v>76.36099999999999</v>
       </c>
       <c r="N37" s="72">
         <v>102.83799999999999</v>
@@ -9283,13 +9283,13 @@
         <v>37.619</v>
       </c>
       <c r="L38" s="72">
-        <v>84.188000000000002</v>
+        <v>84.187999999999988</v>
       </c>
       <c r="M38" s="72">
         <v>18.649999999999999</v>
       </c>
       <c r="N38" s="72">
-        <v>121.807</v>
+        <v>121.80699999999999</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -9324,16 +9324,16 @@
         <v>70</v>
       </c>
       <c r="K39" s="72">
-        <v>25.440999999999999</v>
+        <v>25.441000000000003</v>
       </c>
       <c r="L39" s="72">
-        <v>106.66099999999997</v>
+        <v>106.661</v>
       </c>
       <c r="M39" s="72">
-        <v>15.145999999999999</v>
+        <v>15.146000000000001</v>
       </c>
       <c r="N39" s="72">
-        <v>132.10199999999998</v>
+        <v>132.102</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -9374,7 +9374,7 @@
         <v>102.44799999999999</v>
       </c>
       <c r="M40" s="72">
-        <v>29.654</v>
+        <v>29.654000000000003</v>
       </c>
       <c r="N40" s="72">
         <v>115.22499999999999</v>
@@ -9576,16 +9576,16 @@
         <v>70</v>
       </c>
       <c r="K45" s="72">
-        <v>37.186999999999998</v>
+        <v>37.187000000000005</v>
       </c>
       <c r="L45" s="72">
-        <v>81.470999999999989</v>
+        <v>81.471000000000004</v>
       </c>
       <c r="M45" s="72">
         <v>10.182</v>
       </c>
       <c r="N45" s="72">
-        <v>118.65799999999999</v>
+        <v>118.65800000000002</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -9623,13 +9623,13 @@
         <v>38.667000000000002</v>
       </c>
       <c r="L46" s="72">
-        <v>61.272999999999996</v>
+        <v>61.273000000000025</v>
       </c>
       <c r="M46" s="72">
-        <v>57.384999999999998</v>
+        <v>57.385000000000005</v>
       </c>
       <c r="N46" s="72">
-        <v>99.94</v>
+        <v>99.940000000000026</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -9664,16 +9664,16 @@
         <v>70</v>
       </c>
       <c r="K47" s="72">
-        <v>42.838000000000008</v>
+        <v>42.838000000000001</v>
       </c>
       <c r="L47" s="72">
-        <v>80.270999999999987</v>
+        <v>80.271000000000015</v>
       </c>
       <c r="M47" s="72">
-        <v>19.668999999999997</v>
+        <v>19.669</v>
       </c>
       <c r="N47" s="72">
-        <v>123.10899999999999</v>
+        <v>123.10900000000001</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -9708,10 +9708,10 @@
         <v>70</v>
       </c>
       <c r="K48" s="72">
-        <v>39.658999999999992</v>
+        <v>39.659000000000006</v>
       </c>
       <c r="L48" s="72">
-        <v>98.751000000000005</v>
+        <v>98.750999999999991</v>
       </c>
       <c r="M48" s="72">
         <v>24.357999999999997</v>
@@ -9828,7 +9828,7 @@
         <v>70</v>
       </c>
       <c r="K51" s="72">
-        <v>96.757999999999996</v>
+        <v>96.75800000000001</v>
       </c>
       <c r="L51" s="72">
         <v>0</v>
@@ -9837,7 +9837,7 @@
         <v>0</v>
       </c>
       <c r="N51" s="72">
-        <v>96.757999999999996</v>
+        <v>96.75800000000001</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -9872,7 +9872,7 @@
         <v>70</v>
       </c>
       <c r="K52" s="72">
-        <v>21.166</v>
+        <v>21.166000000000004</v>
       </c>
       <c r="L52" s="72">
         <v>86.775000000000006</v>
@@ -9916,16 +9916,16 @@
         <v>70</v>
       </c>
       <c r="K53" s="72">
-        <v>29.279</v>
+        <v>29.279000000000003</v>
       </c>
       <c r="L53" s="72">
-        <v>99.117000000000019</v>
+        <v>99.11699999999999</v>
       </c>
       <c r="M53" s="72">
         <v>8.8239999999999998</v>
       </c>
       <c r="N53" s="72">
-        <v>128.39600000000002</v>
+        <v>128.39599999999999</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -9963,13 +9963,13 @@
         <v>37.481000000000002</v>
       </c>
       <c r="L54" s="72">
-        <v>102.32800000000003</v>
+        <v>102.328</v>
       </c>
       <c r="M54" s="72">
-        <v>26.067999999999998</v>
+        <v>26.068000000000001</v>
       </c>
       <c r="N54" s="72">
-        <v>139.80900000000003</v>
+        <v>139.809</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -14750,7 +14750,7 @@
         <v>18.706</v>
       </c>
       <c r="M166" s="72">
-        <v>13.532000000000002</v>
+        <v>13.532</v>
       </c>
       <c r="N166" s="72">
         <v>20.744</v>
@@ -14908,10 +14908,10 @@
         <v>70</v>
       </c>
       <c r="K170" s="72">
-        <v>34.121000000000002</v>
+        <v>34.120999999999995</v>
       </c>
       <c r="L170" s="72">
-        <v>48.131000000000007</v>
+        <v>48.131000000000014</v>
       </c>
       <c r="M170" s="72">
         <v>5.2480000000000002</v>
@@ -14996,7 +14996,7 @@
         <v>70</v>
       </c>
       <c r="K172" s="72">
-        <v>18.738999999999997</v>
+        <v>18.739000000000004</v>
       </c>
       <c r="L172" s="72">
         <v>22.963999999999999</v>
@@ -15005,7 +15005,7 @@
         <v>56.864000000000004</v>
       </c>
       <c r="N172" s="72">
-        <v>41.702999999999996</v>
+        <v>41.703000000000003</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
@@ -15040,16 +15040,16 @@
         <v>70</v>
       </c>
       <c r="K173" s="72">
-        <v>18.056000000000001</v>
+        <v>18.055999999999997</v>
       </c>
       <c r="L173" s="72">
-        <v>33.322000000000003</v>
+        <v>33.32200000000001</v>
       </c>
       <c r="M173" s="72">
         <v>8.3810000000000002</v>
       </c>
       <c r="N173" s="72">
-        <v>51.378</v>
+        <v>51.378000000000007</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
@@ -15131,13 +15131,13 @@
         <v>1.8160000000000001</v>
       </c>
       <c r="L175" s="72">
-        <v>23.135000000000002</v>
+        <v>23.134999999999998</v>
       </c>
       <c r="M175" s="72">
         <v>18.701000000000001</v>
       </c>
       <c r="N175" s="72">
-        <v>24.951000000000001</v>
+        <v>24.950999999999997</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
@@ -15175,7 +15175,7 @@
         <v>0</v>
       </c>
       <c r="M176" s="72">
-        <v>24.951000000000001</v>
+        <v>24.950999999999997</v>
       </c>
       <c r="N176" s="72">
         <v>0</v>
@@ -15292,16 +15292,16 @@
         <v>70</v>
       </c>
       <c r="K179" s="72">
-        <v>8.3529999999999998</v>
+        <v>8.3530000000000015</v>
       </c>
       <c r="L179" s="72">
-        <v>47.514000000000003</v>
+        <v>47.513999999999989</v>
       </c>
       <c r="M179" s="72">
         <v>14.751999999999999</v>
       </c>
       <c r="N179" s="72">
-        <v>55.867000000000004</v>
+        <v>55.86699999999999</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.25">
@@ -15386,7 +15386,7 @@
         <v>12.855</v>
       </c>
       <c r="M181" s="72">
-        <v>25.678000000000001</v>
+        <v>25.678000000000004</v>
       </c>
       <c r="N181" s="72">
         <v>30.658000000000001</v>
@@ -15474,7 +15474,7 @@
         <v>33.721000000000004</v>
       </c>
       <c r="M183" s="72">
-        <v>7.7669999999999995</v>
+        <v>7.7670000000000003</v>
       </c>
       <c r="N183" s="72">
         <v>47.858000000000004</v>
@@ -15515,13 +15515,13 @@
         <v>2.6159999999999997</v>
       </c>
       <c r="L184" s="72">
-        <v>26.284999999999997</v>
+        <v>26.285</v>
       </c>
       <c r="M184" s="72">
-        <v>21.573</v>
+        <v>21.572999999999997</v>
       </c>
       <c r="N184" s="72">
-        <v>28.900999999999996</v>
+        <v>28.901</v>
       </c>
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.25">
@@ -15559,7 +15559,7 @@
         <v>0</v>
       </c>
       <c r="M185" s="72">
-        <v>28.900999999999996</v>
+        <v>28.901</v>
       </c>
       <c r="N185" s="72">
         <v>0</v>
@@ -15588,7 +15588,7 @@
         <v>70</v>
       </c>
       <c r="K186" s="72">
-        <v>27.369999999999997</v>
+        <v>27.37</v>
       </c>
       <c r="L186" s="72">
         <v>0</v>
@@ -15597,7 +15597,7 @@
         <v>0</v>
       </c>
       <c r="N186" s="72">
-        <v>27.369999999999997</v>
+        <v>27.37</v>
       </c>
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.25">
@@ -15682,7 +15682,7 @@
         <v>47.315000000000012</v>
       </c>
       <c r="M188" s="72">
-        <v>10.867000000000001</v>
+        <v>10.866999999999999</v>
       </c>
       <c r="N188" s="72">
         <v>75.455000000000013</v>
@@ -15720,13 +15720,13 @@
         <v>70</v>
       </c>
       <c r="K189" s="72">
-        <v>22.33</v>
+        <v>22.330000000000002</v>
       </c>
       <c r="L189" s="72">
         <v>50.837000000000003</v>
       </c>
       <c r="M189" s="72">
-        <v>24.617999999999995</v>
+        <v>24.618000000000002</v>
       </c>
       <c r="N189" s="72">
         <v>73.167000000000002</v>
@@ -16019,13 +16019,13 @@
         <v>29.567</v>
       </c>
       <c r="L196" s="72">
-        <v>22.070999999999998</v>
+        <v>22.071000000000005</v>
       </c>
       <c r="M196" s="72">
         <v>2.6259999999999999</v>
       </c>
       <c r="N196" s="72">
-        <v>51.637999999999998</v>
+        <v>51.638000000000005</v>
       </c>
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.25">
@@ -21128,7 +21128,7 @@
         <v>70</v>
       </c>
       <c r="K316" s="72">
-        <v>81.414000000000001</v>
+        <v>81.414000000000016</v>
       </c>
       <c r="L316" s="72">
         <v>34.913999999999987</v>
@@ -21137,7 +21137,7 @@
         <v>5.0340000000000007</v>
       </c>
       <c r="N316" s="72">
-        <v>116.32799999999999</v>
+        <v>116.328</v>
       </c>
     </row>
     <row r="317" spans="1:14" x14ac:dyDescent="0.25">
@@ -21178,7 +21178,7 @@
         <v>68.215000000000003</v>
       </c>
       <c r="M317" s="72">
-        <v>48.113</v>
+        <v>48.113000000000007</v>
       </c>
       <c r="N317" s="72">
         <v>108.527</v>
@@ -21219,13 +21219,13 @@
         <v>32.225999999999999</v>
       </c>
       <c r="L318" s="72">
-        <v>45.365000000000009</v>
+        <v>45.364999999999981</v>
       </c>
       <c r="M318" s="72">
         <v>63.162000000000006</v>
       </c>
       <c r="N318" s="72">
-        <v>77.591000000000008</v>
+        <v>77.59099999999998</v>
       </c>
     </row>
     <row r="319" spans="1:14" x14ac:dyDescent="0.25">
@@ -21263,13 +21263,13 @@
         <v>38.31</v>
       </c>
       <c r="L319" s="72">
-        <v>61.272000000000006</v>
+        <v>61.271999999999991</v>
       </c>
       <c r="M319" s="72">
-        <v>16.319000000000003</v>
+        <v>16.318999999999999</v>
       </c>
       <c r="N319" s="72">
-        <v>99.582000000000008</v>
+        <v>99.581999999999994</v>
       </c>
     </row>
     <row r="320" spans="1:14" x14ac:dyDescent="0.25">
@@ -21310,7 +21310,7 @@
         <v>29.515000000000008</v>
       </c>
       <c r="M320" s="72">
-        <v>70.066999999999993</v>
+        <v>70.067000000000007</v>
       </c>
       <c r="N320" s="72">
         <v>34.451000000000008</v>
@@ -21427,13 +21427,13 @@
         <v>83.376000000000005</v>
       </c>
       <c r="L323" s="72">
-        <v>35.789000000000016</v>
+        <v>35.788999999999987</v>
       </c>
       <c r="M323" s="72">
         <v>5.0229999999999997</v>
       </c>
       <c r="N323" s="72">
-        <v>119.16500000000002</v>
+        <v>119.16499999999999</v>
       </c>
     </row>
     <row r="324" spans="1:14" x14ac:dyDescent="0.25">
@@ -21468,16 +21468,16 @@
         <v>70</v>
       </c>
       <c r="K324" s="72">
-        <v>24.729999999999997</v>
+        <v>24.73</v>
       </c>
       <c r="L324" s="72">
-        <v>67.988</v>
+        <v>67.987999999999985</v>
       </c>
       <c r="M324" s="72">
-        <v>51.176999999999992</v>
+        <v>51.177000000000007</v>
       </c>
       <c r="N324" s="72">
-        <v>92.718000000000004</v>
+        <v>92.717999999999989</v>
       </c>
     </row>
     <row r="325" spans="1:14" x14ac:dyDescent="0.25">
@@ -21518,7 +21518,7 @@
         <v>29.450999999999993</v>
       </c>
       <c r="M325" s="72">
-        <v>63.267000000000003</v>
+        <v>63.266999999999996</v>
       </c>
       <c r="N325" s="72">
         <v>61.677999999999997</v>
@@ -21676,7 +21676,7 @@
         <v>70</v>
       </c>
       <c r="K329" s="72">
-        <v>41.172000000000004</v>
+        <v>41.171999999999997</v>
       </c>
       <c r="L329" s="72">
         <v>0</v>
@@ -21685,7 +21685,7 @@
         <v>0</v>
       </c>
       <c r="N329" s="72">
-        <v>41.172000000000004</v>
+        <v>41.171999999999997</v>
       </c>
     </row>
     <row r="330" spans="1:14" x14ac:dyDescent="0.25">
@@ -21720,10 +21720,10 @@
         <v>70</v>
       </c>
       <c r="K330" s="72">
-        <v>83.712000000000003</v>
+        <v>83.711999999999989</v>
       </c>
       <c r="L330" s="72">
-        <v>36.189999999999984</v>
+        <v>36.19</v>
       </c>
       <c r="M330" s="72">
         <v>4.9819999999999993</v>
@@ -21767,13 +21767,13 @@
         <v>32.417000000000002</v>
       </c>
       <c r="L331" s="72">
-        <v>67.169999999999987</v>
+        <v>67.170000000000016</v>
       </c>
       <c r="M331" s="72">
         <v>52.731999999999999</v>
       </c>
       <c r="N331" s="72">
-        <v>99.586999999999989</v>
+        <v>99.587000000000018</v>
       </c>
     </row>
     <row r="332" spans="1:14" x14ac:dyDescent="0.25">
@@ -25700,16 +25700,16 @@
         <v>70</v>
       </c>
       <c r="K424" s="72">
-        <v>47.805999999999997</v>
+        <v>47.806000000000004</v>
       </c>
       <c r="L424" s="72">
-        <v>48.184000000000012</v>
+        <v>48.18399999999999</v>
       </c>
       <c r="M424" s="72">
         <v>21.805</v>
       </c>
       <c r="N424" s="72">
-        <v>95.990000000000009</v>
+        <v>95.99</v>
       </c>
     </row>
     <row r="425" spans="1:14" x14ac:dyDescent="0.25">
@@ -25867,13 +25867,13 @@
         <v>85.027999999999992</v>
       </c>
       <c r="L428" s="72">
-        <v>35.53</v>
+        <v>35.530000000000015</v>
       </c>
       <c r="M428" s="72">
         <v>4.9960000000000004</v>
       </c>
       <c r="N428" s="72">
-        <v>120.55799999999999</v>
+        <v>120.55800000000001</v>
       </c>
     </row>
     <row r="429" spans="1:14" x14ac:dyDescent="0.25">
@@ -25908,13 +25908,13 @@
         <v>70</v>
       </c>
       <c r="K429" s="72">
-        <v>33.091000000000008</v>
+        <v>33.091000000000001</v>
       </c>
       <c r="L429" s="72">
-        <v>62.921999999999997</v>
+        <v>62.922000000000004</v>
       </c>
       <c r="M429" s="72">
-        <v>57.635999999999996</v>
+        <v>57.636000000000003</v>
       </c>
       <c r="N429" s="72">
         <v>96.013000000000005</v>
@@ -25996,13 +25996,13 @@
         <v>70</v>
       </c>
       <c r="K431" s="72">
-        <v>32.405999999999999</v>
+        <v>32.406000000000006</v>
       </c>
       <c r="L431" s="72">
-        <v>41.592000000000006</v>
+        <v>41.591999999999999</v>
       </c>
       <c r="M431" s="72">
-        <v>23.436999999999998</v>
+        <v>23.437000000000001</v>
       </c>
       <c r="N431" s="72">
         <v>73.998000000000005</v>
@@ -26043,13 +26043,13 @@
         <v>4.7</v>
       </c>
       <c r="L432" s="72">
-        <v>21.571999999999999</v>
+        <v>21.572000000000003</v>
       </c>
       <c r="M432" s="72">
         <v>52.426000000000002</v>
       </c>
       <c r="N432" s="72">
-        <v>26.271999999999998</v>
+        <v>26.272000000000002</v>
       </c>
     </row>
     <row r="433" spans="1:14" x14ac:dyDescent="0.25">
@@ -26087,7 +26087,7 @@
         <v>0</v>
       </c>
       <c r="M433" s="72">
-        <v>26.271999999999998</v>
+        <v>26.272000000000002</v>
       </c>
       <c r="N433" s="72">
         <v>0</v>
@@ -26116,7 +26116,7 @@
         <v>70</v>
       </c>
       <c r="K434" s="72">
-        <v>37.598999999999997</v>
+        <v>37.599000000000004</v>
       </c>
       <c r="L434" s="72">
         <v>0</v>
@@ -26125,7 +26125,7 @@
         <v>0</v>
       </c>
       <c r="N434" s="72">
-        <v>37.598999999999997</v>
+        <v>37.599000000000004</v>
       </c>
     </row>
     <row r="435" spans="1:14" x14ac:dyDescent="0.25">
@@ -26160,10 +26160,10 @@
         <v>70</v>
       </c>
       <c r="K435" s="72">
-        <v>77.934999999999988</v>
+        <v>77.935000000000002</v>
       </c>
       <c r="L435" s="72">
-        <v>32.616</v>
+        <v>32.615999999999985</v>
       </c>
       <c r="M435" s="72">
         <v>4.9830000000000005</v>
@@ -26204,16 +26204,16 @@
         <v>70</v>
       </c>
       <c r="K436" s="72">
-        <v>35.170999999999999</v>
+        <v>35.170999999999992</v>
       </c>
       <c r="L436" s="72">
-        <v>62.677000000000014</v>
+        <v>62.677000000000007</v>
       </c>
       <c r="M436" s="72">
-        <v>47.874000000000002</v>
+        <v>47.873999999999995</v>
       </c>
       <c r="N436" s="72">
-        <v>97.848000000000013</v>
+        <v>97.847999999999999</v>
       </c>
     </row>
     <row r="437" spans="1:14" x14ac:dyDescent="0.25">
@@ -26251,13 +26251,13 @@
         <v>29.984999999999999</v>
       </c>
       <c r="L437" s="72">
-        <v>29.420999999999999</v>
+        <v>29.420999999999992</v>
       </c>
       <c r="M437" s="72">
-        <v>68.427000000000007</v>
+        <v>68.426999999999992</v>
       </c>
       <c r="N437" s="72">
-        <v>59.405999999999999</v>
+        <v>59.405999999999992</v>
       </c>
     </row>
     <row r="438" spans="1:14" x14ac:dyDescent="0.25">
@@ -26292,16 +26292,16 @@
         <v>70</v>
       </c>
       <c r="K438" s="72">
-        <v>41.431000000000004</v>
+        <v>41.430999999999997</v>
       </c>
       <c r="L438" s="72">
-        <v>43.656999999999989</v>
+        <v>43.657000000000011</v>
       </c>
       <c r="M438" s="72">
-        <v>15.748999999999999</v>
+        <v>15.749000000000001</v>
       </c>
       <c r="N438" s="72">
-        <v>85.087999999999994</v>
+        <v>85.088000000000008</v>
       </c>
     </row>
     <row r="439" spans="1:14" x14ac:dyDescent="0.25">
@@ -26339,13 +26339,13 @@
         <v>4.5459999999999994</v>
       </c>
       <c r="L439" s="72">
-        <v>24.852000000000004</v>
+        <v>24.852</v>
       </c>
       <c r="M439" s="72">
         <v>60.236000000000004</v>
       </c>
       <c r="N439" s="72">
-        <v>29.398000000000003</v>
+        <v>29.398</v>
       </c>
     </row>
     <row r="440" spans="1:14" x14ac:dyDescent="0.25">
@@ -26412,7 +26412,7 @@
         <v>70</v>
       </c>
       <c r="K441" s="72">
-        <v>35.077000000000005</v>
+        <v>35.076999999999998</v>
       </c>
       <c r="L441" s="72">
         <v>0</v>
@@ -26421,7 +26421,7 @@
         <v>0</v>
       </c>
       <c r="N441" s="72">
-        <v>35.077000000000005</v>
+        <v>35.076999999999998</v>
       </c>
     </row>
     <row r="442" spans="1:14" x14ac:dyDescent="0.25">
@@ -26459,13 +26459,13 @@
         <v>71.494</v>
       </c>
       <c r="L442" s="72">
-        <v>30.138999999999982</v>
+        <v>30.13900000000001</v>
       </c>
       <c r="M442" s="72">
         <v>4.9380000000000006</v>
       </c>
       <c r="N442" s="72">
-        <v>101.63299999999998</v>
+        <v>101.63300000000001</v>
       </c>
     </row>
     <row r="443" spans="1:14" x14ac:dyDescent="0.25">
@@ -30222,7 +30222,7 @@
         <v>25.972999999999999</v>
       </c>
       <c r="M531" s="72">
-        <v>60.487000000000009</v>
+        <v>60.486999999999995</v>
       </c>
       <c r="N531" s="72">
         <v>30.6</v>
@@ -30336,10 +30336,10 @@
         <v>70</v>
       </c>
       <c r="K534" s="72">
-        <v>43.604000000000006</v>
+        <v>43.603999999999999</v>
       </c>
       <c r="L534" s="72">
-        <v>37.249000000000002</v>
+        <v>37.249000000000009</v>
       </c>
       <c r="M534" s="72">
         <v>4.8019999999999996</v>
@@ -30380,13 +30380,13 @@
         <v>70</v>
       </c>
       <c r="K535" s="72">
-        <v>80.176000000000002</v>
+        <v>80.175999999999988</v>
       </c>
       <c r="L535" s="72">
-        <v>8.3199999999999932</v>
+        <v>8.3200000000000074</v>
       </c>
       <c r="M535" s="72">
-        <v>72.533000000000001</v>
+        <v>72.533000000000015</v>
       </c>
       <c r="N535" s="72">
         <v>88.495999999999995</v>
@@ -30427,13 +30427,13 @@
         <v>4.5339999999999998</v>
       </c>
       <c r="L536" s="72">
-        <v>26.398000000000003</v>
+        <v>26.398</v>
       </c>
       <c r="M536" s="72">
         <v>62.097999999999992</v>
       </c>
       <c r="N536" s="72">
-        <v>30.932000000000002</v>
+        <v>30.931999999999999</v>
       </c>
     </row>
     <row r="537" spans="1:14" x14ac:dyDescent="0.25">
@@ -30471,7 +30471,7 @@
         <v>0</v>
       </c>
       <c r="M537" s="72">
-        <v>30.932000000000002</v>
+        <v>30.931999999999999</v>
       </c>
       <c r="N537" s="72">
         <v>0</v>
@@ -30594,7 +30594,7 @@
         <v>8.2870000000000061</v>
       </c>
       <c r="M540" s="72">
-        <v>79.15300000000002</v>
+        <v>79.152999999999992</v>
       </c>
       <c r="N540" s="72">
         <v>80.472000000000008</v>
@@ -30635,13 +30635,13 @@
         <v>4.484</v>
       </c>
       <c r="L541" s="72">
-        <v>24.045999999999992</v>
+        <v>24.045999999999999</v>
       </c>
       <c r="M541" s="72">
         <v>56.426000000000002</v>
       </c>
       <c r="N541" s="72">
-        <v>28.529999999999994</v>
+        <v>28.53</v>
       </c>
     </row>
     <row r="542" spans="1:14" x14ac:dyDescent="0.25">
@@ -30679,7 +30679,7 @@
         <v>0</v>
       </c>
       <c r="M542" s="72">
-        <v>28.529999999999994</v>
+        <v>28.53</v>
       </c>
       <c r="N542" s="72">
         <v>0</v>
@@ -30708,7 +30708,7 @@
         <v>70</v>
       </c>
       <c r="K543" s="72">
-        <v>41.298999999999999</v>
+        <v>41.299000000000007</v>
       </c>
       <c r="L543" s="72">
         <v>0</v>
@@ -30717,7 +30717,7 @@
         <v>0</v>
       </c>
       <c r="N543" s="72">
-        <v>41.298999999999999</v>
+        <v>41.299000000000007</v>
       </c>
     </row>
     <row r="544" spans="1:14" x14ac:dyDescent="0.25">
@@ -30755,13 +30755,13 @@
         <v>42.210999999999999</v>
       </c>
       <c r="L544" s="72">
-        <v>36.558999999999983</v>
+        <v>36.559000000000012</v>
       </c>
       <c r="M544" s="72">
         <v>4.74</v>
       </c>
       <c r="N544" s="72">
-        <v>78.769999999999982</v>
+        <v>78.77000000000001</v>
       </c>
     </row>
     <row r="545" spans="1:14" x14ac:dyDescent="0.25">
@@ -33500,16 +33500,16 @@
         <v>70</v>
       </c>
       <c r="K610" s="72">
-        <v>72.176000000000002</v>
+        <v>72.176000000000016</v>
       </c>
       <c r="L610" s="72">
-        <v>11.834000000000017</v>
+        <v>11.833999999999975</v>
       </c>
       <c r="M610" s="72">
-        <v>111.49400000000001</v>
+        <v>111.494</v>
       </c>
       <c r="N610" s="72">
-        <v>84.010000000000019</v>
+        <v>84.009999999999991</v>
       </c>
     </row>
     <row r="611" spans="1:14" x14ac:dyDescent="0.25">
@@ -33664,16 +33664,16 @@
         <v>70</v>
       </c>
       <c r="K614" s="72">
-        <v>88.594000000000008</v>
+        <v>88.593999999999994</v>
       </c>
       <c r="L614" s="72">
-        <v>37.853999999999999</v>
+        <v>37.854000000000028</v>
       </c>
       <c r="M614" s="72">
         <v>4.6050000000000004</v>
       </c>
       <c r="N614" s="72">
-        <v>126.44800000000001</v>
+        <v>126.44800000000002</v>
       </c>
     </row>
     <row r="615" spans="1:14" x14ac:dyDescent="0.25">
@@ -33711,13 +33711,13 @@
         <v>66.293999999999997</v>
       </c>
       <c r="L615" s="72">
-        <v>11.719999999999985</v>
+        <v>11.719999999999999</v>
       </c>
       <c r="M615" s="72">
         <v>114.72800000000001</v>
       </c>
       <c r="N615" s="72">
-        <v>78.013999999999982</v>
+        <v>78.013999999999996</v>
       </c>
     </row>
     <row r="616" spans="1:14" x14ac:dyDescent="0.25">
@@ -33755,13 +33755,13 @@
         <v>2.3449999999999998</v>
       </c>
       <c r="L616" s="72">
-        <v>23.707999999999998</v>
+        <v>23.708000000000002</v>
       </c>
       <c r="M616" s="72">
-        <v>54.306000000000004</v>
+        <v>54.305999999999997</v>
       </c>
       <c r="N616" s="72">
-        <v>26.052999999999997</v>
+        <v>26.053000000000001</v>
       </c>
     </row>
     <row r="617" spans="1:14" x14ac:dyDescent="0.25">
@@ -33799,7 +33799,7 @@
         <v>0</v>
       </c>
       <c r="M617" s="72">
-        <v>26.052999999999997</v>
+        <v>26.053000000000001</v>
       </c>
       <c r="N617" s="72">
         <v>0</v>
@@ -33919,13 +33919,13 @@
         <v>62.125</v>
       </c>
       <c r="L620" s="72">
-        <v>11.673000000000002</v>
+        <v>11.672999999999973</v>
       </c>
       <c r="M620" s="72">
         <v>117.51900000000001</v>
       </c>
       <c r="N620" s="72">
-        <v>73.798000000000002</v>
+        <v>73.797999999999973</v>
       </c>
     </row>
     <row r="621" spans="1:14" x14ac:dyDescent="0.25">
@@ -33966,7 +33966,7 @@
         <v>22.518999999999998</v>
       </c>
       <c r="M621" s="72">
-        <v>51.278999999999996</v>
+        <v>51.279000000000003</v>
       </c>
       <c r="N621" s="72">
         <v>24.838999999999999</v>
@@ -34036,7 +34036,7 @@
         <v>70</v>
       </c>
       <c r="K623" s="72">
-        <v>40.553999999999995</v>
+        <v>40.554000000000002</v>
       </c>
       <c r="L623" s="72">
         <v>0</v>
@@ -34045,7 +34045,7 @@
         <v>0</v>
       </c>
       <c r="N623" s="72">
-        <v>40.553999999999995</v>
+        <v>40.554000000000002</v>
       </c>
     </row>
     <row r="624" spans="1:14" x14ac:dyDescent="0.25">
@@ -34080,10 +34080,10 @@
         <v>70</v>
       </c>
       <c r="K624" s="72">
-        <v>83.218000000000004</v>
+        <v>83.217999999999989</v>
       </c>
       <c r="L624" s="72">
-        <v>36.007999999999996</v>
+        <v>36.00800000000001</v>
       </c>
       <c r="M624" s="72">
         <v>4.5459999999999994</v>
@@ -37095,13 +37095,13 @@
         <v>45.114000000000004</v>
       </c>
       <c r="L696" s="72">
-        <v>40.292999999999978</v>
+        <v>40.293000000000006</v>
       </c>
       <c r="M696" s="72">
         <v>10.637</v>
       </c>
       <c r="N696" s="72">
-        <v>85.406999999999982</v>
+        <v>85.407000000000011</v>
       </c>
     </row>
     <row r="697" spans="1:14" x14ac:dyDescent="0.25">
@@ -37142,10 +37142,10 @@
         <v>25.673999999999999</v>
       </c>
       <c r="M697" s="72">
-        <v>59.73299999999999</v>
+        <v>59.733000000000004</v>
       </c>
       <c r="N697" s="72">
-        <v>30.785999999999998</v>
+        <v>30.786000000000001</v>
       </c>
     </row>
     <row r="698" spans="1:14" x14ac:dyDescent="0.25">
@@ -37183,7 +37183,7 @@
         <v>0</v>
       </c>
       <c r="M698" s="72">
-        <v>30.785999999999998</v>
+        <v>30.786000000000001</v>
       </c>
       <c r="N698" s="72">
         <v>0</v>
@@ -37256,16 +37256,16 @@
         <v>70</v>
       </c>
       <c r="K700" s="72">
-        <v>84.49799999999999</v>
+        <v>84.498000000000019</v>
       </c>
       <c r="L700" s="72">
-        <v>36.315000000000012</v>
+        <v>36.314999999999969</v>
       </c>
       <c r="M700" s="72">
         <v>5.1010000000000009</v>
       </c>
       <c r="N700" s="72">
-        <v>120.813</v>
+        <v>120.81299999999999</v>
       </c>
     </row>
     <row r="701" spans="1:14" x14ac:dyDescent="0.25">
@@ -37300,7 +37300,7 @@
         <v>70</v>
       </c>
       <c r="K701" s="72">
-        <v>48.096000000000004</v>
+        <v>48.095999999999997</v>
       </c>
       <c r="L701" s="72">
         <v>69.959000000000003</v>
@@ -37347,13 +37347,13 @@
         <v>21.003999999999998</v>
       </c>
       <c r="L702" s="72">
-        <v>31.041000000000004</v>
+        <v>31.040999999999997</v>
       </c>
       <c r="M702" s="72">
-        <v>87.013999999999996</v>
+        <v>87.01400000000001</v>
       </c>
       <c r="N702" s="72">
-        <v>52.045000000000002</v>
+        <v>52.044999999999995</v>
       </c>
     </row>
     <row r="703" spans="1:14" x14ac:dyDescent="0.25">
@@ -37388,16 +37388,16 @@
         <v>70</v>
       </c>
       <c r="K703" s="72">
-        <v>45.569999999999993</v>
+        <v>45.570000000000007</v>
       </c>
       <c r="L703" s="72">
-        <v>41.64800000000001</v>
+        <v>41.647999999999982</v>
       </c>
       <c r="M703" s="72">
-        <v>10.396999999999998</v>
+        <v>10.397</v>
       </c>
       <c r="N703" s="72">
-        <v>87.218000000000004</v>
+        <v>87.217999999999989</v>
       </c>
     </row>
     <row r="704" spans="1:14" x14ac:dyDescent="0.25">
@@ -37435,13 +37435,13 @@
         <v>4.9969999999999999</v>
       </c>
       <c r="L704" s="72">
-        <v>26.094000000000001</v>
+        <v>26.093999999999998</v>
       </c>
       <c r="M704" s="72">
         <v>61.123999999999995</v>
       </c>
       <c r="N704" s="72">
-        <v>31.091000000000001</v>
+        <v>31.090999999999998</v>
       </c>
     </row>
     <row r="705" spans="1:14" x14ac:dyDescent="0.25">
@@ -37479,7 +37479,7 @@
         <v>0</v>
       </c>
       <c r="M705" s="72">
-        <v>31.091000000000001</v>
+        <v>31.090999999999998</v>
       </c>
       <c r="N705" s="72">
         <v>0</v>
@@ -37508,7 +37508,7 @@
         <v>70</v>
       </c>
       <c r="K706" s="72">
-        <v>40.457000000000008</v>
+        <v>40.457000000000001</v>
       </c>
       <c r="L706" s="72">
         <v>0</v>
@@ -37517,7 +37517,7 @@
         <v>0</v>
       </c>
       <c r="N706" s="72">
-        <v>40.457000000000008</v>
+        <v>40.457000000000001</v>
       </c>
     </row>
     <row r="707" spans="1:14" x14ac:dyDescent="0.25">
@@ -37552,10 +37552,10 @@
         <v>70</v>
       </c>
       <c r="K707" s="72">
-        <v>82.228999999999999</v>
+        <v>82.229000000000013</v>
       </c>
       <c r="L707" s="72">
-        <v>35.362000000000009</v>
+        <v>35.361999999999995</v>
       </c>
       <c r="M707" s="72">
         <v>5.0950000000000006</v>
@@ -37599,13 +37599,13 @@
         <v>50.183</v>
       </c>
       <c r="L708" s="72">
-        <v>75.40900000000002</v>
+        <v>75.408999999999992</v>
       </c>
       <c r="M708" s="72">
         <v>42.182000000000002</v>
       </c>
       <c r="N708" s="72">
-        <v>125.59200000000001</v>
+        <v>125.59199999999998</v>
       </c>
     </row>
     <row r="709" spans="1:14" x14ac:dyDescent="0.25">
@@ -37640,16 +37640,16 @@
         <v>70</v>
       </c>
       <c r="K709" s="72">
-        <v>21.181000000000001</v>
+        <v>21.180999999999997</v>
       </c>
       <c r="L709" s="72">
-        <v>33.805999999999997</v>
+        <v>33.806000000000004</v>
       </c>
       <c r="M709" s="72">
         <v>91.786000000000001</v>
       </c>
       <c r="N709" s="72">
-        <v>54.986999999999995</v>
+        <v>54.987000000000002</v>
       </c>
     </row>
     <row r="710" spans="1:14" x14ac:dyDescent="0.25">
@@ -37731,13 +37731,13 @@
         <v>4.9260000000000002</v>
       </c>
       <c r="L711" s="72">
-        <v>23.654000000000003</v>
+        <v>23.653999999999996</v>
       </c>
       <c r="M711" s="72">
         <v>55.442999999999998</v>
       </c>
       <c r="N711" s="72">
-        <v>28.580000000000002</v>
+        <v>28.58</v>
       </c>
     </row>
     <row r="712" spans="1:14" x14ac:dyDescent="0.25">
@@ -37775,7 +37775,7 @@
         <v>0</v>
       </c>
       <c r="M712" s="72">
-        <v>28.580000000000002</v>
+        <v>28.58</v>
       </c>
       <c r="N712" s="72">
         <v>0</v>
@@ -37804,7 +37804,7 @@
         <v>70</v>
       </c>
       <c r="K713" s="72">
-        <v>43.901000000000003</v>
+        <v>43.900999999999996</v>
       </c>
       <c r="L713" s="72">
         <v>0</v>
@@ -37813,7 +37813,7 @@
         <v>0</v>
       </c>
       <c r="N713" s="72">
-        <v>43.901000000000003</v>
+        <v>43.900999999999996</v>
       </c>
     </row>
     <row r="714" spans="1:14" x14ac:dyDescent="0.25">
@@ -37892,16 +37892,16 @@
         <v>70</v>
       </c>
       <c r="K715" s="72">
-        <v>41.241999999999997</v>
+        <v>41.242000000000004</v>
       </c>
       <c r="L715" s="72">
-        <v>69.324999999999989</v>
+        <v>69.325000000000003</v>
       </c>
       <c r="M715" s="72">
         <v>59.378</v>
       </c>
       <c r="N715" s="72">
-        <v>110.56699999999999</v>
+        <v>110.56700000000001</v>
       </c>
     </row>
     <row r="716" spans="1:14" x14ac:dyDescent="0.25">
@@ -37936,10 +37936,10 @@
         <v>70</v>
       </c>
       <c r="K716" s="72">
-        <v>21.017999999999997</v>
+        <v>21.018000000000001</v>
       </c>
       <c r="L716" s="72">
-        <v>27.435000000000006</v>
+        <v>27.435000000000002</v>
       </c>
       <c r="M716" s="72">
         <v>83.132000000000005</v>
@@ -41875,13 +41875,13 @@
         <v>4.9349999999999996</v>
       </c>
       <c r="L809" s="72">
-        <v>27.038999999999998</v>
+        <v>27.039000000000005</v>
       </c>
       <c r="M809" s="72">
-        <v>65.039999999999992</v>
+        <v>65.040000000000006</v>
       </c>
       <c r="N809" s="72">
-        <v>31.973999999999997</v>
+        <v>31.974000000000004</v>
       </c>
     </row>
     <row r="810" spans="1:14" x14ac:dyDescent="0.25">
@@ -41919,7 +41919,7 @@
         <v>0</v>
       </c>
       <c r="M810" s="72">
-        <v>31.973999999999997</v>
+        <v>31.974000000000004</v>
       </c>
       <c r="N810" s="72">
         <v>0</v>
@@ -41992,16 +41992,16 @@
         <v>70</v>
       </c>
       <c r="K812" s="72">
-        <v>81.776999999999987</v>
+        <v>81.777000000000015</v>
       </c>
       <c r="L812" s="72">
-        <v>34.184000000000026</v>
+        <v>34.183999999999983</v>
       </c>
       <c r="M812" s="72">
         <v>4.9450000000000003</v>
       </c>
       <c r="N812" s="72">
-        <v>115.96100000000001</v>
+        <v>115.961</v>
       </c>
     </row>
     <row r="813" spans="1:14" x14ac:dyDescent="0.25">
@@ -42036,13 +42036,13 @@
         <v>70</v>
       </c>
       <c r="K813" s="72">
-        <v>58.760999999999996</v>
+        <v>58.76100000000001</v>
       </c>
       <c r="L813" s="72">
-        <v>70.724999999999994</v>
+        <v>70.72499999999998</v>
       </c>
       <c r="M813" s="72">
-        <v>45.235999999999997</v>
+        <v>45.23599999999999</v>
       </c>
       <c r="N813" s="72">
         <v>129.48599999999999</v>
@@ -42083,13 +42083,13 @@
         <v>22.163</v>
       </c>
       <c r="L814" s="72">
-        <v>46.44</v>
+        <v>46.440000000000012</v>
       </c>
       <c r="M814" s="72">
         <v>83.045999999999992</v>
       </c>
       <c r="N814" s="72">
-        <v>68.602999999999994</v>
+        <v>68.603000000000009</v>
       </c>
     </row>
     <row r="815" spans="1:14" x14ac:dyDescent="0.25">
@@ -42124,13 +42124,13 @@
         <v>70</v>
       </c>
       <c r="K815" s="72">
-        <v>27.510999999999999</v>
+        <v>27.511000000000003</v>
       </c>
       <c r="L815" s="72">
-        <v>52.846000000000004</v>
+        <v>52.845999999999997</v>
       </c>
       <c r="M815" s="72">
-        <v>15.757</v>
+        <v>15.757000000000001</v>
       </c>
       <c r="N815" s="72">
         <v>80.356999999999999</v>
@@ -42244,7 +42244,7 @@
         <v>70</v>
       </c>
       <c r="K818" s="72">
-        <v>40.885999999999996</v>
+        <v>40.88600000000001</v>
       </c>
       <c r="L818" s="72">
         <v>0</v>
@@ -42253,7 +42253,7 @@
         <v>0</v>
       </c>
       <c r="N818" s="72">
-        <v>40.885999999999996</v>
+        <v>40.88600000000001</v>
       </c>
     </row>
     <row r="819" spans="1:14" x14ac:dyDescent="0.25">
@@ -42288,10 +42288,10 @@
         <v>70</v>
       </c>
       <c r="K819" s="72">
-        <v>85.801000000000002</v>
+        <v>85.800999999999988</v>
       </c>
       <c r="L819" s="72">
-        <v>35.946000000000012</v>
+        <v>35.946000000000026</v>
       </c>
       <c r="M819" s="72">
         <v>4.9399999999999995</v>
@@ -42332,13 +42332,13 @@
         <v>70</v>
       </c>
       <c r="K820" s="72">
-        <v>50.12700000000001</v>
+        <v>50.127000000000002</v>
       </c>
       <c r="L820" s="72">
         <v>70.575999999999993</v>
       </c>
       <c r="M820" s="72">
-        <v>51.170999999999999</v>
+        <v>51.170999999999992</v>
       </c>
       <c r="N820" s="72">
         <v>120.703</v>
@@ -42379,13 +42379,13 @@
         <v>22.951999999999998</v>
       </c>
       <c r="L821" s="72">
-        <v>33.570000000000007</v>
+        <v>33.57</v>
       </c>
       <c r="M821" s="72">
-        <v>87.132999999999996</v>
+        <v>87.13300000000001</v>
       </c>
       <c r="N821" s="72">
-        <v>56.522000000000006</v>
+        <v>56.521999999999998</v>
       </c>
     </row>
     <row r="822" spans="1:14" x14ac:dyDescent="0.25">
@@ -42420,16 +42420,16 @@
         <v>70</v>
       </c>
       <c r="K822" s="72">
-        <v>31.288000000000004</v>
+        <v>31.288</v>
       </c>
       <c r="L822" s="72">
-        <v>43.143999999999984</v>
+        <v>43.144000000000005</v>
       </c>
       <c r="M822" s="72">
         <v>13.378</v>
       </c>
       <c r="N822" s="72">
-        <v>74.431999999999988</v>
+        <v>74.432000000000002</v>
       </c>
     </row>
     <row r="823" spans="1:14" x14ac:dyDescent="0.25">
@@ -42467,13 +42467,13 @@
         <v>4.7549999999999999</v>
       </c>
       <c r="L823" s="72">
-        <v>21.765000000000001</v>
+        <v>21.764999999999997</v>
       </c>
       <c r="M823" s="72">
         <v>52.667000000000002</v>
       </c>
       <c r="N823" s="72">
-        <v>26.52</v>
+        <v>26.519999999999996</v>
       </c>
     </row>
     <row r="824" spans="1:14" x14ac:dyDescent="0.25">
@@ -42511,7 +42511,7 @@
         <v>0</v>
       </c>
       <c r="M824" s="72">
-        <v>26.52</v>
+        <v>26.519999999999996</v>
       </c>
       <c r="N824" s="72">
         <v>0</v>
@@ -42540,7 +42540,7 @@
         <v>70</v>
       </c>
       <c r="K825" s="72">
-        <v>38.227000000000004</v>
+        <v>38.226999999999997</v>
       </c>
       <c r="L825" s="72">
         <v>0</v>
@@ -42549,7 +42549,7 @@
         <v>0</v>
       </c>
       <c r="N825" s="72">
-        <v>38.227000000000004</v>
+        <v>38.226999999999997</v>
       </c>
     </row>
     <row r="826" spans="1:14" x14ac:dyDescent="0.25">
@@ -42631,13 +42631,13 @@
         <v>53.33</v>
       </c>
       <c r="L827" s="72">
-        <v>70.082999999999998</v>
+        <v>70.083000000000013</v>
       </c>
       <c r="M827" s="72">
         <v>42.518999999999998</v>
       </c>
       <c r="N827" s="72">
-        <v>123.413</v>
+        <v>123.41300000000001</v>
       </c>
     </row>
     <row r="828" spans="1:14" x14ac:dyDescent="0.25">
@@ -42672,16 +42672,16 @@
         <v>70</v>
       </c>
       <c r="K828" s="72">
-        <v>22.078000000000003</v>
+        <v>22.077999999999999</v>
       </c>
       <c r="L828" s="72">
         <v>39.036000000000001</v>
       </c>
       <c r="M828" s="72">
-        <v>84.376999999999981</v>
+        <v>84.37700000000001</v>
       </c>
       <c r="N828" s="72">
-        <v>61.114000000000004</v>
+        <v>61.113999999999997</v>
       </c>
     </row>
     <row r="829" spans="1:14" x14ac:dyDescent="0.25">
@@ -46356,7 +46356,7 @@
         <v>70</v>
       </c>
       <c r="K915" s="72">
-        <v>19.269000000000005</v>
+        <v>19.269000000000002</v>
       </c>
       <c r="L915" s="72">
         <v>32.852999999999994</v>
@@ -46365,7 +46365,7 @@
         <v>65.289000000000001</v>
       </c>
       <c r="N915" s="72">
-        <v>52.122</v>
+        <v>52.121999999999993</v>
       </c>
     </row>
     <row r="916" spans="1:14" x14ac:dyDescent="0.25">
@@ -46400,10 +46400,10 @@
         <v>70</v>
       </c>
       <c r="K916" s="72">
-        <v>21.110999999999997</v>
+        <v>21.111000000000004</v>
       </c>
       <c r="L916" s="72">
-        <v>41.258000000000003</v>
+        <v>41.257999999999996</v>
       </c>
       <c r="M916" s="72">
         <v>10.864000000000001</v>
@@ -46447,13 +46447,13 @@
         <v>38.295000000000002</v>
       </c>
       <c r="L917" s="72">
-        <v>50.971999999999994</v>
+        <v>50.972000000000008</v>
       </c>
       <c r="M917" s="72">
         <v>11.397</v>
       </c>
       <c r="N917" s="72">
-        <v>89.266999999999996</v>
+        <v>89.26700000000001</v>
       </c>
     </row>
     <row r="918" spans="1:14" x14ac:dyDescent="0.25">
@@ -46494,7 +46494,7 @@
         <v>40.075000000000003</v>
       </c>
       <c r="M918" s="72">
-        <v>49.191999999999993</v>
+        <v>49.192</v>
       </c>
       <c r="N918" s="72">
         <v>44.887</v>
@@ -46608,16 +46608,16 @@
         <v>70</v>
       </c>
       <c r="K921" s="72">
-        <v>58.700999999999993</v>
+        <v>58.701000000000008</v>
       </c>
       <c r="L921" s="72">
-        <v>48.461000000000013</v>
+        <v>48.46099999999997</v>
       </c>
       <c r="M921" s="72">
         <v>4.6939999999999991</v>
       </c>
       <c r="N921" s="72">
-        <v>107.16200000000001</v>
+        <v>107.16199999999998</v>
       </c>
     </row>
     <row r="922" spans="1:14" x14ac:dyDescent="0.25">
@@ -46658,7 +46658,7 @@
         <v>85.785999999999987</v>
       </c>
       <c r="M922" s="72">
-        <v>21.376000000000001</v>
+        <v>21.375999999999998</v>
       </c>
       <c r="N922" s="72">
         <v>123.30199999999999</v>
@@ -46696,10 +46696,10 @@
         <v>70</v>
       </c>
       <c r="K923" s="72">
-        <v>34.152999999999999</v>
+        <v>34.153000000000006</v>
       </c>
       <c r="L923" s="72">
-        <v>86.927000000000021</v>
+        <v>86.927000000000007</v>
       </c>
       <c r="M923" s="72">
         <v>36.375</v>
@@ -46784,16 +46784,16 @@
         <v>70</v>
       </c>
       <c r="K925" s="72">
-        <v>25.044999999999998</v>
+        <v>25.045000000000002</v>
       </c>
       <c r="L925" s="72">
-        <v>48.911999999999992</v>
+        <v>48.912000000000006</v>
       </c>
       <c r="M925" s="72">
-        <v>12.003</v>
+        <v>12.002999999999998</v>
       </c>
       <c r="N925" s="72">
-        <v>73.956999999999994</v>
+        <v>73.957000000000008</v>
       </c>
     </row>
     <row r="926" spans="1:14" x14ac:dyDescent="0.25">
@@ -46878,7 +46878,7 @@
         <v>34.726999999999997</v>
       </c>
       <c r="M927" s="72">
-        <v>42.494</v>
+        <v>42.494000000000007</v>
       </c>
       <c r="N927" s="72">
         <v>39.155999999999999</v>
@@ -46995,13 +46995,13 @@
         <v>61.225000000000001</v>
       </c>
       <c r="L930" s="72">
-        <v>50.896999999999998</v>
+        <v>50.897000000000013</v>
       </c>
       <c r="M930" s="72">
         <v>4.6720000000000006</v>
       </c>
       <c r="N930" s="72">
-        <v>112.122</v>
+        <v>112.12200000000001</v>
       </c>
     </row>
     <row r="931" spans="1:14" x14ac:dyDescent="0.25">
@@ -47039,13 +47039,13 @@
         <v>28.707000000000001</v>
       </c>
       <c r="L931" s="72">
-        <v>74.373000000000019</v>
+        <v>74.37299999999999</v>
       </c>
       <c r="M931" s="72">
-        <v>37.749000000000002</v>
+        <v>37.748999999999995</v>
       </c>
       <c r="N931" s="72">
-        <v>103.08000000000001</v>
+        <v>103.07999999999998</v>
       </c>
     </row>
     <row r="932" spans="1:14" x14ac:dyDescent="0.25">
@@ -47080,16 +47080,16 @@
         <v>70</v>
       </c>
       <c r="K932" s="72">
-        <v>26.821000000000005</v>
+        <v>26.821000000000002</v>
       </c>
       <c r="L932" s="72">
-        <v>67.072000000000003</v>
+        <v>67.072000000000017</v>
       </c>
       <c r="M932" s="72">
-        <v>36.007999999999996</v>
+        <v>36.008000000000003</v>
       </c>
       <c r="N932" s="72">
-        <v>93.893000000000001</v>
+        <v>93.893000000000015</v>
       </c>
     </row>
     <row r="933" spans="1:14" x14ac:dyDescent="0.25">
@@ -50287,13 +50287,13 @@
         <v>30.01</v>
       </c>
       <c r="L1007" s="72">
-        <v>120.42600000000003</v>
+        <v>120.426</v>
       </c>
       <c r="M1007" s="72">
-        <v>22.187999999999999</v>
+        <v>22.188000000000002</v>
       </c>
       <c r="N1007" s="72">
-        <v>150.43600000000004</v>
+        <v>150.43600000000001</v>
       </c>
     </row>
     <row r="1008" spans="1:14" x14ac:dyDescent="0.25">
@@ -50451,13 +50451,13 @@
         <v>58.872</v>
       </c>
       <c r="L1011" s="72">
-        <v>46.714000000000013</v>
+        <v>46.713999999999999</v>
       </c>
       <c r="M1011" s="72">
         <v>4.6259999999999994</v>
       </c>
       <c r="N1011" s="72">
-        <v>105.58600000000001</v>
+        <v>105.586</v>
       </c>
     </row>
     <row r="1012" spans="1:14" x14ac:dyDescent="0.25">
@@ -50492,7 +50492,7 @@
         <v>70</v>
       </c>
       <c r="K1012" s="72">
-        <v>24.227</v>
+        <v>24.226999999999997</v>
       </c>
       <c r="L1012" s="72">
         <v>85.88</v>
@@ -50536,16 +50536,16 @@
         <v>70</v>
       </c>
       <c r="K1013" s="72">
-        <v>31.74</v>
+        <v>31.740000000000002</v>
       </c>
       <c r="L1013" s="72">
-        <v>72.568000000000026</v>
+        <v>72.567999999999984</v>
       </c>
       <c r="M1013" s="72">
         <v>37.539000000000001</v>
       </c>
       <c r="N1013" s="72">
-        <v>104.30800000000002</v>
+        <v>104.30799999999999</v>
       </c>
     </row>
     <row r="1014" spans="1:14" x14ac:dyDescent="0.25">
@@ -50624,10 +50624,10 @@
         <v>70</v>
       </c>
       <c r="K1015" s="72">
-        <v>30.844999999999999</v>
+        <v>30.845000000000006</v>
       </c>
       <c r="L1015" s="72">
-        <v>50.753999999999991</v>
+        <v>50.753999999999984</v>
       </c>
       <c r="M1015" s="72">
         <v>11.545999999999999</v>
@@ -50671,13 +50671,13 @@
         <v>17.427</v>
       </c>
       <c r="L1016" s="72">
-        <v>60.352999999999987</v>
+        <v>60.353000000000002</v>
       </c>
       <c r="M1016" s="72">
         <v>21.246000000000002</v>
       </c>
       <c r="N1016" s="72">
-        <v>77.779999999999987</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="1017" spans="1:14" x14ac:dyDescent="0.25">
@@ -50832,16 +50832,16 @@
         <v>70</v>
       </c>
       <c r="K1020" s="72">
-        <v>58.657999999999987</v>
+        <v>58.658000000000001</v>
       </c>
       <c r="L1020" s="72">
-        <v>47.03700000000002</v>
+        <v>47.036999999999992</v>
       </c>
       <c r="M1020" s="72">
         <v>4.4610000000000003</v>
       </c>
       <c r="N1020" s="72">
-        <v>105.69500000000001</v>
+        <v>105.69499999999999</v>
       </c>
     </row>
     <row r="1021" spans="1:14" x14ac:dyDescent="0.25">
@@ -50920,7 +50920,7 @@
         <v>70</v>
       </c>
       <c r="K1022" s="72">
-        <v>34.549000000000007</v>
+        <v>34.548999999999999</v>
       </c>
       <c r="L1022" s="72">
         <v>85.844999999999999</v>
@@ -50967,13 +50967,13 @@
         <v>25.271000000000001</v>
       </c>
       <c r="L1023" s="72">
-        <v>41.813000000000002</v>
+        <v>41.812999999999988</v>
       </c>
       <c r="M1023" s="72">
-        <v>78.581000000000017</v>
+        <v>78.580999999999989</v>
       </c>
       <c r="N1023" s="72">
-        <v>67.084000000000003</v>
+        <v>67.083999999999989</v>
       </c>
     </row>
     <row r="1024" spans="1:14" x14ac:dyDescent="0.25">
@@ -54540,7 +54540,7 @@
         <v>70</v>
       </c>
       <c r="K1107" s="72">
-        <v>24.462000000000003</v>
+        <v>24.462</v>
       </c>
       <c r="L1107" s="72">
         <v>118.211</v>
@@ -54751,13 +54751,13 @@
         <v>11.416</v>
       </c>
       <c r="L1112" s="72">
-        <v>87.013999999999982</v>
+        <v>87.01400000000001</v>
       </c>
       <c r="M1112" s="72">
-        <v>30.247999999999998</v>
+        <v>30.248000000000005</v>
       </c>
       <c r="N1112" s="72">
-        <v>98.429999999999978</v>
+        <v>98.43</v>
       </c>
     </row>
     <row r="1113" spans="1:14" x14ac:dyDescent="0.25">
@@ -54795,13 +54795,13 @@
         <v>10.905999999999999</v>
       </c>
       <c r="L1113" s="72">
-        <v>52.375999999999998</v>
+        <v>52.376000000000012</v>
       </c>
       <c r="M1113" s="72">
         <v>46.054000000000002</v>
       </c>
       <c r="N1113" s="72">
-        <v>63.281999999999996</v>
+        <v>63.282000000000011</v>
       </c>
     </row>
     <row r="1114" spans="1:14" x14ac:dyDescent="0.25">
@@ -54839,7 +54839,7 @@
         <v>0</v>
       </c>
       <c r="M1114" s="72">
-        <v>63.281999999999996</v>
+        <v>63.282000000000011</v>
       </c>
       <c r="N1114" s="72">
         <v>0</v>
@@ -54868,7 +54868,7 @@
         <v>70</v>
       </c>
       <c r="K1115" s="72">
-        <v>108.80900000000001</v>
+        <v>108.809</v>
       </c>
       <c r="L1115" s="72">
         <v>0</v>
@@ -54877,7 +54877,7 @@
         <v>0</v>
       </c>
       <c r="N1115" s="72">
-        <v>108.80900000000001</v>
+        <v>108.809</v>
       </c>
     </row>
     <row r="1116" spans="1:14" x14ac:dyDescent="0.25">
@@ -54915,13 +54915,13 @@
         <v>25.219000000000001</v>
       </c>
       <c r="L1116" s="72">
-        <v>101.40600000000003</v>
+        <v>101.40600000000001</v>
       </c>
       <c r="M1116" s="72">
         <v>7.4030000000000005</v>
       </c>
       <c r="N1116" s="72">
-        <v>126.62500000000003</v>
+        <v>126.625</v>
       </c>
     </row>
     <row r="1117" spans="1:14" x14ac:dyDescent="0.25">
@@ -56878,7 +56878,7 @@
         <v>15.121000000000002</v>
       </c>
       <c r="M1163" s="72">
-        <v>12.488999999999999</v>
+        <v>12.489000000000001</v>
       </c>
       <c r="N1163" s="72">
         <v>17.103000000000002</v>
@@ -57156,7 +57156,7 @@
         <v>70</v>
       </c>
       <c r="K1170" s="72">
-        <v>36.894999999999996</v>
+        <v>36.895000000000003</v>
       </c>
       <c r="L1170" s="72">
         <v>0</v>
@@ -57165,7 +57165,7 @@
         <v>0</v>
       </c>
       <c r="N1170" s="72">
-        <v>36.894999999999996</v>
+        <v>36.895000000000003</v>
       </c>
     </row>
     <row r="1171" spans="1:14" x14ac:dyDescent="0.25">
@@ -57203,13 +57203,13 @@
         <v>4.6769999999999996</v>
       </c>
       <c r="L1171" s="72">
-        <v>29.138000000000005</v>
+        <v>29.137999999999998</v>
       </c>
       <c r="M1171" s="72">
         <v>7.7569999999999997</v>
       </c>
       <c r="N1171" s="72">
-        <v>33.815000000000005</v>
+        <v>33.814999999999998</v>
       </c>
     </row>
     <row r="1172" spans="1:14" x14ac:dyDescent="0.25">
@@ -57247,13 +57247,13 @@
         <v>2.1219999999999999</v>
       </c>
       <c r="L1172" s="72">
-        <v>21.026000000000003</v>
+        <v>21.026</v>
       </c>
       <c r="M1172" s="72">
         <v>12.789</v>
       </c>
       <c r="N1172" s="72">
-        <v>23.148000000000003</v>
+        <v>23.148</v>
       </c>
     </row>
     <row r="1173" spans="1:14" x14ac:dyDescent="0.25">
@@ -61571,13 +61571,13 @@
         <v>0</v>
       </c>
       <c r="G6" s="72">
-        <v>258.13924999999989</v>
+        <v>258.13925000000006</v>
       </c>
       <c r="H6" s="72">
         <v>350</v>
       </c>
       <c r="I6" s="76">
-        <v>0.73754071428571399</v>
+        <v>0.73754071428571444</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -61600,13 +61600,13 @@
         <v>0</v>
       </c>
       <c r="G7" s="72">
-        <v>46.930250000000015</v>
+        <v>46.930250000000001</v>
       </c>
       <c r="H7" s="72">
         <v>350</v>
       </c>
       <c r="I7" s="76">
-        <v>0.13408642857142861</v>
+        <v>0.13408642857142858</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -61687,13 +61687,13 @@
         <v>0</v>
       </c>
       <c r="G10" s="72">
-        <v>296.44324999999975</v>
+        <v>296.44324999999998</v>
       </c>
       <c r="H10" s="72">
         <v>350</v>
       </c>
       <c r="I10" s="76">
-        <v>0.84698071428571353</v>
+        <v>0.8469807142857142</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -61716,13 +61716,13 @@
         <v>0</v>
       </c>
       <c r="G11" s="72">
-        <v>76.063999999999993</v>
+        <v>76.064000000000021</v>
       </c>
       <c r="H11" s="72">
         <v>350</v>
       </c>
       <c r="I11" s="76">
-        <v>0.21732571428571426</v>
+        <v>0.21732571428571434</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -61803,13 +61803,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="72">
-        <v>80.989750000000029</v>
+        <v>80.989750000000015</v>
       </c>
       <c r="H14" s="72">
         <v>140</v>
       </c>
       <c r="I14" s="76">
-        <v>0.57849821428571446</v>
+        <v>0.57849821428571435</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -61832,13 +61832,13 @@
         <v>0</v>
       </c>
       <c r="G15" s="72">
-        <v>103.20675000000006</v>
+        <v>103.20675</v>
       </c>
       <c r="H15" s="72">
         <v>140</v>
       </c>
       <c r="I15" s="76">
-        <v>0.73719107142857188</v>
+        <v>0.73719107142857143</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -61861,13 +61861,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="72">
-        <v>418.61849999999987</v>
+        <v>418.61849999999993</v>
       </c>
       <c r="H16" s="72">
         <v>490</v>
       </c>
       <c r="I16" s="76">
-        <v>0.85432346938775483</v>
+        <v>0.85432346938775494</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -61890,13 +61890,13 @@
         <v>0</v>
       </c>
       <c r="G17" s="72">
-        <v>156.1815</v>
+        <v>156.18149999999983</v>
       </c>
       <c r="H17" s="72">
         <v>490</v>
       </c>
       <c r="I17" s="76">
-        <v>0.31873775510204083</v>
+        <v>0.31873775510204044</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -61919,13 +61919,13 @@
         <v>0</v>
       </c>
       <c r="G18" s="72">
-        <v>40.9</v>
+        <v>40.900000000000006</v>
       </c>
       <c r="H18" s="72">
         <v>140</v>
       </c>
       <c r="I18" s="76">
-        <v>0.29214285714285715</v>
+        <v>0.2921428571428572</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -62093,13 +62093,13 @@
         <v>0</v>
       </c>
       <c r="G24" s="72">
-        <v>61.135749999999987</v>
+        <v>61.135750000000016</v>
       </c>
       <c r="H24" s="72">
         <v>210</v>
       </c>
       <c r="I24" s="76">
-        <v>0.29112261904761899</v>
+        <v>0.2911226190476191</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -62122,13 +62122,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="72">
-        <v>43.853500000000004</v>
+        <v>43.853500000000018</v>
       </c>
       <c r="H25" s="72">
         <v>210</v>
       </c>
       <c r="I25" s="76">
-        <v>0.2088261904761905</v>
+        <v>0.20882619047619055</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -62209,13 +62209,13 @@
         <v>0</v>
       </c>
       <c r="G28" s="72">
-        <v>178.53650000000005</v>
+        <v>178.53650000000002</v>
       </c>
       <c r="H28" s="72">
         <v>210</v>
       </c>
       <c r="I28" s="76">
-        <v>0.85017380952380972</v>
+        <v>0.85017380952380961</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -62238,7 +62238,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="72">
-        <v>126.28975000000004</v>
+        <v>126.28975000000003</v>
       </c>
       <c r="H29" s="72">
         <v>210</v>
@@ -62325,13 +62325,13 @@
         <v>0</v>
       </c>
       <c r="G32" s="72">
-        <v>121.27874999999996</v>
+        <v>121.27875000000006</v>
       </c>
       <c r="H32" s="72">
         <v>210</v>
       </c>
       <c r="I32" s="76">
-        <v>0.57751785714285697</v>
+        <v>0.57751785714285742</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -62354,13 +62354,13 @@
         <v>0</v>
       </c>
       <c r="G33" s="72">
-        <v>175.43350000000004</v>
+        <v>175.43349999999992</v>
       </c>
       <c r="H33" s="72">
         <v>210</v>
       </c>
       <c r="I33" s="76">
-        <v>0.83539761904761922</v>
+        <v>0.83539761904761867</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -62383,13 +62383,13 @@
         <v>0</v>
       </c>
       <c r="G34" s="72">
-        <v>724.85199999999907</v>
+        <v>724.85199999999952</v>
       </c>
       <c r="H34" s="72">
         <v>910</v>
       </c>
       <c r="I34" s="76">
-        <v>0.79654065934065832</v>
+        <v>0.79654065934065876</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -62615,13 +62615,13 @@
         <v>0</v>
       </c>
       <c r="G42" s="72">
-        <v>64.462499999999935</v>
+        <v>64.462500000000048</v>
       </c>
       <c r="H42" s="72">
         <v>210</v>
       </c>
       <c r="I42" s="76">
-        <v>0.30696428571428541</v>
+        <v>0.30696428571428597</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -62644,13 +62644,13 @@
         <v>0</v>
       </c>
       <c r="G43" s="72">
-        <v>38.313249999999996</v>
+        <v>38.313250000000032</v>
       </c>
       <c r="H43" s="72">
         <v>210</v>
       </c>
       <c r="I43" s="76">
-        <v>0.18244404761904759</v>
+        <v>0.18244404761904778</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -62731,13 +62731,13 @@
         <v>0</v>
       </c>
       <c r="G46" s="72">
-        <v>124.24325000000003</v>
+        <v>124.24324999999988</v>
       </c>
       <c r="H46" s="72">
         <v>210</v>
       </c>
       <c r="I46" s="76">
-        <v>0.59163452380952397</v>
+        <v>0.59163452380952319</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -62760,13 +62760,13 @@
         <v>0</v>
       </c>
       <c r="G47" s="72">
-        <v>114.32925000000009</v>
+        <v>114.32925000000004</v>
       </c>
       <c r="H47" s="72">
         <v>210</v>
       </c>
       <c r="I47" s="76">
-        <v>0.54442500000000038</v>
+        <v>0.54442500000000016</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -62847,13 +62847,13 @@
         <v>0</v>
       </c>
       <c r="G50" s="72">
-        <v>124.49675000000006</v>
+        <v>124.49674999999992</v>
       </c>
       <c r="H50" s="72">
         <v>210</v>
       </c>
       <c r="I50" s="76">
-        <v>0.59284166666666693</v>
+        <v>0.59284166666666627</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -62876,13 +62876,13 @@
         <v>0</v>
       </c>
       <c r="G51" s="72">
-        <v>188.66499999999996</v>
+        <v>188.66499999999994</v>
       </c>
       <c r="H51" s="72">
         <v>210</v>
       </c>
       <c r="I51" s="76">
-        <v>0.89840476190476171</v>
+        <v>0.8984047619047616</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -62905,13 +62905,13 @@
         <v>0</v>
       </c>
       <c r="G52" s="72">
-        <v>413.38475</v>
+        <v>413.38474999999983</v>
       </c>
       <c r="H52" s="72">
         <v>770</v>
       </c>
       <c r="I52" s="76">
-        <v>0.5368633116883117</v>
+        <v>0.53686331168831147</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -62934,13 +62934,13 @@
         <v>0</v>
       </c>
       <c r="G53" s="72">
-        <v>525.06875000000014</v>
+        <v>525.06874999999991</v>
       </c>
       <c r="H53" s="72">
         <v>770</v>
       </c>
       <c r="I53" s="76">
-        <v>0.68190746753246767</v>
+        <v>0.68190746753246745</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -62963,13 +62963,13 @@
         <v>0</v>
       </c>
       <c r="G54" s="72">
-        <v>43.967250000000021</v>
+        <v>43.967249999999986</v>
       </c>
       <c r="H54" s="72">
         <v>210</v>
       </c>
       <c r="I54" s="76">
-        <v>0.20936785714285724</v>
+        <v>0.20936785714285708</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -63137,13 +63137,13 @@
         <v>0</v>
       </c>
       <c r="G60" s="72">
-        <v>62.991000000000007</v>
+        <v>62.991000000000035</v>
       </c>
       <c r="H60" s="72">
         <v>210</v>
       </c>
       <c r="I60" s="76">
-        <v>0.29995714285714287</v>
+        <v>0.29995714285714303</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -63166,13 +63166,13 @@
         <v>0</v>
       </c>
       <c r="G61" s="72">
-        <v>42.273750000000007</v>
+        <v>42.27375</v>
       </c>
       <c r="H61" s="72">
         <v>210</v>
       </c>
       <c r="I61" s="76">
-        <v>0.20130357142857147</v>
+        <v>0.20130357142857142</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -63253,13 +63253,13 @@
         <v>0</v>
       </c>
       <c r="G64" s="72">
-        <v>183.98975000000007</v>
+        <v>183.9897499999999</v>
       </c>
       <c r="H64" s="72">
         <v>210</v>
       </c>
       <c r="I64" s="76">
-        <v>0.87614166666666704</v>
+        <v>0.87614166666666615</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -63369,13 +63369,13 @@
         <v>0</v>
       </c>
       <c r="G68" s="72">
-        <v>128.22175000000001</v>
+        <v>128.22175000000004</v>
       </c>
       <c r="H68" s="72">
         <v>210</v>
       </c>
       <c r="I68" s="76">
-        <v>0.61057976190476193</v>
+        <v>0.61057976190476215</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -63427,13 +63427,13 @@
         <v>0</v>
       </c>
       <c r="G70" s="72">
-        <v>263.18924999999996</v>
+        <v>263.1892499999999</v>
       </c>
       <c r="H70" s="72">
         <v>350</v>
       </c>
       <c r="I70" s="76">
-        <v>0.75196928571428556</v>
+        <v>0.75196928571428545</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -63456,13 +63456,13 @@
         <v>0</v>
       </c>
       <c r="G71" s="72">
-        <v>219.71574999999999</v>
+        <v>219.71575000000004</v>
       </c>
       <c r="H71" s="72">
         <v>350</v>
       </c>
       <c r="I71" s="76">
-        <v>0.62775928571428563</v>
+        <v>0.62775928571428585</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -63485,13 +63485,13 @@
         <v>0</v>
       </c>
       <c r="G72" s="72">
-        <v>45.395250000000019</v>
+        <v>45.395250000000004</v>
       </c>
       <c r="H72" s="72">
         <v>210</v>
       </c>
       <c r="I72" s="76">
-        <v>0.21616785714285724</v>
+        <v>0.21616785714285716</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -63514,13 +63514,13 @@
         <v>0</v>
       </c>
       <c r="G73" s="72">
-        <v>56.677999999999997</v>
+        <v>56.678000000000011</v>
       </c>
       <c r="H73" s="72">
         <v>210</v>
       </c>
       <c r="I73" s="76">
-        <v>0.26989523809523808</v>
+        <v>0.26989523809523813</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -63688,13 +63688,13 @@
         <v>0</v>
       </c>
       <c r="G79" s="72">
-        <v>35.89</v>
+        <v>35.889999999999993</v>
       </c>
       <c r="H79" s="72">
         <v>140</v>
       </c>
       <c r="I79" s="76">
-        <v>0.25635714285714284</v>
+        <v>0.25635714285714278</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -63717,13 +63717,13 @@
         <v>0</v>
       </c>
       <c r="G80" s="72">
-        <v>110.01474999999996</v>
+        <v>110.01474999999995</v>
       </c>
       <c r="H80" s="72">
         <v>140</v>
       </c>
       <c r="I80" s="76">
-        <v>0.78581964285714256</v>
+        <v>0.78581964285714245</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -63775,13 +63775,13 @@
         <v>0</v>
       </c>
       <c r="G82" s="72">
-        <v>192.11725000000004</v>
+        <v>192.11724999999996</v>
       </c>
       <c r="H82" s="72">
         <v>210</v>
       </c>
       <c r="I82" s="76">
-        <v>0.91484404761904781</v>
+        <v>0.91484404761904736</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -63804,13 +63804,13 @@
         <v>0</v>
       </c>
       <c r="G83" s="72">
-        <v>86.186750000000004</v>
+        <v>86.186750000000046</v>
       </c>
       <c r="H83" s="72">
         <v>210</v>
       </c>
       <c r="I83" s="76">
-        <v>0.41041309523809527</v>
+        <v>0.41041309523809544</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -63833,13 +63833,13 @@
         <v>0</v>
       </c>
       <c r="G84" s="72">
-        <v>168.25125000000003</v>
+        <v>168.25125000000008</v>
       </c>
       <c r="H84" s="72">
         <v>210</v>
       </c>
       <c r="I84" s="76">
-        <v>0.8011964285714287</v>
+        <v>0.80119642857142892</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -63862,13 +63862,13 @@
         <v>0</v>
       </c>
       <c r="G85" s="72">
-        <v>40.551999999999978</v>
+        <v>40.552</v>
       </c>
       <c r="H85" s="72">
         <v>210</v>
       </c>
       <c r="I85" s="76">
-        <v>0.19310476190476181</v>
+        <v>0.19310476190476189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>